<commit_message>
Fixed bugs causing heap corruption
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shirl\source\repos\PANDA-original\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shirl\source\repos\PANDA_POSSUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6493036A-E078-4FB6-9BB3-668D761259C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78963CC-286B-4168-9BD4-290F568873B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10725" yWindow="1500" windowWidth="14025" windowHeight="14055"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="inputsetup" sheetId="1" r:id="rId1"/>
+    <sheet name="inputsetup" sheetId="3" r:id="rId1"/>
     <sheet name="weighttable" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t>Weight</t>
   </si>
@@ -48,12 +49,159 @@
   </si>
   <si>
     <t>PaddlerCentre</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Lf</t>
+  </si>
+  <si>
+    <t>Ld</t>
+  </si>
+  <si>
+    <t>Lp</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>decreasing section size</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>member ID</t>
+  </si>
+  <si>
+    <t>section group</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>1 (bottom)</t>
+  </si>
+  <si>
+    <t>2 (mid)</t>
+  </si>
+  <si>
+    <t>3 (top)</t>
+  </si>
+  <si>
+    <t>include triple, double, single</t>
+  </si>
+  <si>
+    <t>section groups in order of decreasing stiffness</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V1, V2, V3</t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>==</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>THEN</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!= </t>
+  </si>
+  <si>
+    <t>double X</t>
+  </si>
+  <si>
+    <t>panel group</t>
+  </si>
+  <si>
+    <t>panel ID</t>
+  </si>
+  <si>
+    <t>PATTERNS</t>
+  </si>
+  <si>
+    <t>MANUAL CONSTRAINT DEFINITIONS</t>
+  </si>
+  <si>
+    <t>define sections in decreasing stiffness button</t>
+  </si>
+  <si>
+    <t>-&gt; project settings dialog</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>constaint 1</t>
+  </si>
+  <si>
+    <t>constraint 1</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>constraint 2</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>[checkbox]</t>
+  </si>
+  <si>
+    <t>------&gt;</t>
+  </si>
+  <si>
+    <t>table</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -190,7 +338,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,8 +518,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -483,6 +643,160 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,8 +845,31 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -887,11 +1224,213 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE74D95-DAEA-4914-80C7-F037AFDBAFC4}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>5.2</v>
+      </c>
+      <c r="C2">
+        <v>5.7</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="C5">
+        <v>1.5</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>0.6</v>
+      </c>
+      <c r="C6">
+        <v>0.7</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>0.35</v>
+      </c>
+      <c r="C9">
+        <v>0.35</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0.2</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0.2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0.17449999999999999</v>
+      </c>
+      <c r="C12">
+        <v>0.17449999999999999</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>0.7</v>
+      </c>
+      <c r="C13">
+        <v>0.9</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,253 +1566,241 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D170F-722C-465D-8093-AB44222604A5}">
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.85546875" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C1">
-        <v>20</v>
-      </c>
-      <c r="D1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="D8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="D9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="D10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="D11" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="16"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>0.6</v>
-      </c>
-      <c r="C2">
-        <v>0.05</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0.2</v>
-      </c>
-      <c r="C3">
-        <v>0.1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0.1</v>
-      </c>
-      <c r="C5">
-        <v>0.05</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1.57</v>
-      </c>
-      <c r="C6">
-        <v>0.78500000000000003</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0.7</v>
-      </c>
-      <c r="C8">
-        <v>0.2</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0.1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>0.6</v>
-      </c>
-      <c r="C10">
-        <v>0.05</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>0.15</v>
-      </c>
-      <c r="C11">
-        <v>0.1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>5</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>0.1</v>
-      </c>
-      <c r="C13">
-        <v>0.05</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14">
-        <v>1.57</v>
-      </c>
-      <c r="C14">
-        <v>0.78500000000000003</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16">
-        <v>0.7</v>
-      </c>
-      <c r="C16">
-        <v>0.2</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0.1</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
+      <c r="B21" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>